<commit_message>
ADD añadido video de nioh 3 y creación de usuarios de los tres roles
</commit_message>
<xml_diff>
--- a/uploads/imports.xlsx
+++ b/uploads/imports.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="55">
   <si>
     <t xml:space="preserve">sku</t>
   </si>
@@ -112,7 +112,7 @@
     <t xml:space="preserve">Prepárate para la acción cooperativa más intensa en Helldrivers 2. Pilota tu vehículo a través de escenarios infernales llenos de enemigos despiadados, explosiones masivas y misiones trepidantes. Con un enfoque en el multijugador cooperativo, progresión de armas y habilidades, y un diseño de niveles frenético, esta secuela promete combates explosivos y diversión sin parar.</t>
   </si>
   <si>
-    <t xml:space="preserve">cover_helldrivers₂.jpg</t>
+    <t xml:space="preserve">cover_helldrivers_2.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Acción,Shooter,Multijugador</t>
@@ -130,7 +130,10 @@
     <t xml:space="preserve">Adéntrate en un Japón feudal lleno de demonios y guerreros en Nioh 3. Domina un sistema de combate profundo y estratégico mientras exploras paisajes impresionantes, te enfrentas a jefes desafiantes y descubres secretos ocultos. Con mecánicas refinadas, personalización de armas y habilidades, y una narrativa inmersiva, Nioh 3 ofrece una experiencia de acción-RPG intensa y gratificante.</t>
   </si>
   <si>
-    <t xml:space="preserve">cover_nioh₃.jpg</t>
+    <t xml:space="preserve">cover_nioh_3.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nioh_3.mp4</t>
   </si>
   <si>
     <t xml:space="preserve">Acción</t>
@@ -270,7 +273,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -291,16 +294,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -437,7 +432,7 @@
   <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J8" activeCellId="0" sqref="J8"/>
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -495,10 +490,10 @@
       <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="O1" s="4" t="s">
         <v>14</v>
       </c>
     </row>
@@ -506,20 +501,20 @@
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6" t="n">
+      <c r="E2" s="5"/>
+      <c r="F2" s="5" t="n">
         <v>70</v>
       </c>
-      <c r="G2" s="6" t="n">
+      <c r="G2" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H2" s="1" t="n">
@@ -531,10 +526,10 @@
       <c r="M2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="N2" s="0" t="s">
+      <c r="N2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="O2" s="6" t="s">
         <v>20</v>
       </c>
     </row>
@@ -542,20 +537,20 @@
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6" t="n">
+      <c r="E3" s="5"/>
+      <c r="F3" s="5" t="n">
         <v>60</v>
       </c>
-      <c r="G3" s="6" t="n">
+      <c r="G3" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H3" s="1" t="n">
@@ -567,10 +562,10 @@
       <c r="M3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="N3" s="0" t="s">
+      <c r="N3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="O3" s="7" t="s">
+      <c r="O3" s="6" t="s">
         <v>26</v>
       </c>
     </row>
@@ -602,10 +597,10 @@
       <c r="M4" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="N4" s="0" t="s">
+      <c r="N4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="O4" s="0" t="s">
+      <c r="O4" s="1" t="s">
         <v>32</v>
       </c>
     </row>
@@ -616,20 +611,23 @@
       <c r="B5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="6" t="s">
         <v>35</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="E5" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="F5" s="1" t="n">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="G5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1" t="n">
         <v>0</v>
-      </c>
-      <c r="H5" s="1" t="n">
-        <v>1</v>
       </c>
       <c r="I5" s="1" t="n">
         <v>10</v>
@@ -637,25 +635,25 @@
       <c r="M5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="N5" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="O5" s="7" t="s">
+      <c r="N5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="O5" s="6" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="8" t="s">
         <v>40</v>
       </c>
+      <c r="C6" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="D6" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F6" s="1" t="n">
         <v>120</v>
@@ -672,25 +670,25 @@
       <c r="M6" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="N6" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="O6" s="0" t="s">
+      <c r="N6" s="1" t="s">
         <v>43</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C7" s="8" t="s">
         <v>46</v>
       </c>
+      <c r="C7" s="6" t="s">
+        <v>47</v>
+      </c>
       <c r="D7" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F7" s="1" t="n">
         <v>20</v>
@@ -707,25 +705,25 @@
       <c r="M7" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="N7" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="O7" s="0" t="s">
-        <v>43</v>
+      <c r="N7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C8" s="8" t="s">
         <v>51</v>
       </c>
+      <c r="C8" s="6" t="s">
+        <v>52</v>
+      </c>
       <c r="D8" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F8" s="1" t="n">
         <v>40</v>
@@ -742,23 +740,23 @@
       <c r="M8" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="N8" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="O8" s="0" t="s">
+      <c r="N8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="O8" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="1"/>
-      <c r="E9" s="8"/>
+      <c r="E9" s="6"/>
       <c r="F9" s="1"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="L13" s="9"/>
+      <c r="L13" s="7"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D18" s="8"/>
+      <c r="D18" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
ADD importar excel con phpspreadsheet
</commit_message>
<xml_diff>
--- a/uploads/imports.xlsx
+++ b/uploads/imports.xlsx
@@ -133,7 +133,7 @@
     <t xml:space="preserve">cover_nioh_3.jpg</t>
   </si>
   <si>
-    <t xml:space="preserve">Nioh_3.mp4</t>
+    <t xml:space="preserve">nioh_3.mp4</t>
   </si>
   <si>
     <t xml:space="preserve">Acción</t>
@@ -273,7 +273,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -299,6 +299,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -432,7 +436,7 @@
   <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -752,8 +756,11 @@
       <c r="E9" s="6"/>
       <c r="F9" s="1"/>
     </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F12" s="7"/>
+    </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="L13" s="7"/>
+      <c r="L13" s="8"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D18" s="6"/>

</xml_diff>

<commit_message>
ADD mkdocs hasta sprint 4
</commit_message>
<xml_diff>
--- a/uploads/imports.xlsx
+++ b/uploads/imports.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
   <si>
     <t xml:space="preserve">sku</t>
   </si>
@@ -118,7 +118,7 @@
     <t xml:space="preserve">Acción,Shooter,Multijugador</t>
   </si>
   <si>
-    <t xml:space="preserve">PC,PlayStation 5,Xbox Series X</t>
+    <t xml:space="preserve">Steam,PlayStation 5,Xbox Series X</t>
   </si>
   <si>
     <t xml:space="preserve">P00014</t>
@@ -139,6 +139,9 @@
     <t xml:space="preserve">Acción</t>
   </si>
   <si>
+    <t xml:space="preserve">Steam,PlayStation 5</t>
+  </si>
+  <si>
     <t xml:space="preserve">P00015</t>
   </si>
   <si>
@@ -154,7 +157,7 @@
     <t xml:space="preserve">Productividad</t>
   </si>
   <si>
-    <t xml:space="preserve">PC</t>
+    <t xml:space="preserve">Software</t>
   </si>
   <si>
     <t xml:space="preserve">P00016</t>
@@ -170,6 +173,9 @@
   </si>
   <si>
     <t xml:space="preserve">Aventura,Indie,Estrategia,Multijugador</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Steam</t>
   </si>
   <si>
     <t xml:space="preserve">P00017</t>
@@ -431,8 +437,8 @@
   </sheetPr>
   <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J17" activeCellId="0" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -448,6 +454,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="14.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="12.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="6.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="24.62"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -639,21 +646,21 @@
         <v>38</v>
       </c>
       <c r="O5" s="6" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F6" s="1" t="n">
         <v>120</v>
@@ -671,24 +678,24 @@
         <v>1</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F7" s="1" t="n">
         <v>20</v>
@@ -706,24 +713,24 @@
         <v>1</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>44</v>
+        <v>50</v>
+      </c>
+      <c r="O7" s="6" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F8" s="1" t="n">
         <v>40</v>
@@ -741,10 +748,10 @@
         <v>1</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>